<commit_message>
geting a student name cours mark and credit and sve ina dictionary
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>First Names</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>Marks</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>third</t>
+  </si>
+  <si>
+    <t>four</t>
   </si>
 </sst>
 </file>
@@ -360,18 +372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -381,6 +393,34 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
geting al students name courses credits and marks and save in a list
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>First Names</t>
   </si>
@@ -29,18 +29,6 @@
   </si>
   <si>
     <t>Marks</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>third</t>
-  </si>
-  <si>
-    <t>four</t>
   </si>
 </sst>
 </file>
@@ -372,18 +360,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -393,34 +381,6 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>65</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>